<commit_message>
added for future use
</commit_message>
<xml_diff>
--- a/node_server/src/services/Medical Data.xlsx
+++ b/node_server/src/services/Medical Data.xlsx
@@ -1,36 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26415"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_FFD2BC37D08E6A056820A83309603D8DF5C3ED45" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0F011A8-8335-4666-9136-262B1E231308}"/>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Patient illnesses 2000 - 2002" sheetId="1" r:id="rId1"/>
-    <sheet name="Physicians missions 2000 - 2002" sheetId="2" r:id="rId2"/>
-    <sheet name="Most bough drugs 2000 - 2002" sheetId="3" r:id="rId3"/>
+    <sheet state="visible" name="Patient illnesses 2000 - 2002" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Physicians missions 2000 - 2002" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Most bough drugs 2000 - 2002" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+  <si>
+    <t>Malaria</t>
+  </si>
+  <si>
+    <t>lyphbia</t>
+  </si>
+  <si>
+    <t>fever</t>
+  </si>
+  <si>
+    <t>Typhoid</t>
+  </si>
+  <si>
+    <t>Neurophobia</t>
+  </si>
+  <si>
+    <t>Diarheaa</t>
+  </si>
+  <si>
+    <t>Hiv</t>
+  </si>
+  <si>
+    <t>tactophoibia</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>lusophobia</t>
+  </si>
+  <si>
+    <t>marasme</t>
+  </si>
   <si>
     <t>Lagos</t>
   </si>
@@ -89,16 +105,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -109,43 +124,44 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -335,192 +351,215 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+    <row r="2">
+      <c r="A2" s="1">
+        <v>2000.0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2001.0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2002.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" s="1">
-        <v>2000</v>
+        <v>2000.0</v>
       </c>
       <c r="B2" s="1">
-        <v>2001</v>
+        <v>2001.0</v>
       </c>
       <c r="C2" s="1">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>2002.0</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2">
       <c r="A2" s="1">
-        <v>2000</v>
+        <v>2000.0</v>
       </c>
       <c r="B2" s="1">
-        <v>2001</v>
+        <v>2001.0</v>
       </c>
       <c r="C2" s="1">
-        <v>2002</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>2002.0</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>